<commit_message>
Correction d'un bug qui créait des doublons de la valeur "Toutes" pour le choix d'années dans le 2eme onglet. Ajout du nombre de reçus dans les onglets Correction bug sauvegarde reçu inexistant dans .save pour les adhérents avec un don régulier sum < min Le statut d'un membre ne passe pas à P&R si la somme du paiement régulier ne dépasse pas le min Il n'y a plus la date de l'édition du reçu dans son hash pour éviter de regénérer tous les jours. + Fonction dédiée. Renommer Receipt.getDict en .getDataDict + arg editionDate True par défaut On peut maintenant trier les deux treeviews Bouton pour ouvrir un reçu Début préparation mail pour Thunderbird
</commit_message>
<xml_diff>
--- a/donnees/listesAdherents/2024.xlsx
+++ b/donnees/listesAdherents/2024.xlsx
@@ -605,7 +605,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>240124NG1;240102NGR1</t>
+          <t>240124NG1</t>
         </is>
       </c>
       <c r="E2" s="2" t="inlineStr">
@@ -614,10 +614,8 @@
         </is>
       </c>
       <c r="F2" s="2" t="n"/>
-      <c r="G2" s="2" t="inlineStr">
-        <is>
-          <t>P&amp;R</t>
-        </is>
+      <c r="G2" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="H2" s="2" t="b">
         <v>1</v>
@@ -686,7 +684,7 @@
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
-          <t>240122NA1;240102NAR1</t>
+          <t>240122NA1</t>
         </is>
       </c>
       <c r="E3" s="2" t="inlineStr">
@@ -695,10 +693,8 @@
         </is>
       </c>
       <c r="F3" s="2" t="n"/>
-      <c r="G3" s="2" t="inlineStr">
-        <is>
-          <t>P&amp;R</t>
-        </is>
+      <c r="G3" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="H3" s="2" t="b">
         <v>1</v>
@@ -1638,20 +1634,14 @@
           <t>Olivia</t>
         </is>
       </c>
-      <c r="D15" s="2" t="inlineStr">
-        <is>
-          <t>240109OPR1</t>
-        </is>
-      </c>
+      <c r="D15" s="2" t="inlineStr"/>
       <c r="E15" s="2" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
       </c>
       <c r="F15" s="2" t="n"/>
-      <c r="G15" s="2" t="b">
-        <v>1</v>
-      </c>
+      <c r="G15" s="2" t="n"/>
       <c r="H15" s="2" t="b">
         <v>1</v>
       </c>
@@ -2434,20 +2424,14 @@
           <t>Moral</t>
         </is>
       </c>
-      <c r="D25" s="2" t="inlineStr">
-        <is>
-          <t>240114MMR1</t>
-        </is>
-      </c>
+      <c r="D25" s="2" t="inlineStr"/>
       <c r="E25" s="2" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
       </c>
       <c r="F25" s="2" t="n"/>
-      <c r="G25" s="2" t="b">
-        <v>1</v>
-      </c>
+      <c r="G25" s="2" t="n"/>
       <c r="H25" s="2" t="b">
         <v>1</v>
       </c>
@@ -3396,20 +3380,14 @@
           <t>Bérangère</t>
         </is>
       </c>
-      <c r="D37" s="2" t="inlineStr">
-        <is>
-          <t>240119BMR1</t>
-        </is>
-      </c>
+      <c r="D37" s="2" t="inlineStr"/>
       <c r="E37" s="2" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
       </c>
       <c r="F37" s="2" t="n"/>
-      <c r="G37" s="2" t="b">
-        <v>1</v>
-      </c>
+      <c r="G37" s="2" t="n"/>
       <c r="H37" s="2" t="b">
         <v>1</v>
       </c>
@@ -3475,20 +3453,14 @@
           <t>Jacques</t>
         </is>
       </c>
-      <c r="D38" s="2" t="inlineStr">
-        <is>
-          <t>240120JJR1</t>
-        </is>
-      </c>
+      <c r="D38" s="2" t="inlineStr"/>
       <c r="E38" s="2" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
       </c>
       <c r="F38" s="2" t="n"/>
-      <c r="G38" s="2" t="b">
-        <v>1</v>
-      </c>
+      <c r="G38" s="2" t="n"/>
       <c r="H38" s="2" t="b">
         <v>1</v>
       </c>
@@ -4348,20 +4320,14 @@
           <t>Therese</t>
         </is>
       </c>
-      <c r="D49" s="2" t="inlineStr">
-        <is>
-          <t>240129TWR1</t>
-        </is>
-      </c>
+      <c r="D49" s="2" t="inlineStr"/>
       <c r="E49" s="2" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
       </c>
       <c r="F49" s="2" t="n"/>
-      <c r="G49" s="2" t="b">
-        <v>1</v>
-      </c>
+      <c r="G49" s="2" t="n"/>
       <c r="H49" s="2" t="b">
         <v>1</v>
       </c>
@@ -4670,20 +4636,14 @@
           <t>Julien</t>
         </is>
       </c>
-      <c r="D53" s="2" t="inlineStr">
-        <is>
-          <t>240131JBR1</t>
-        </is>
-      </c>
+      <c r="D53" s="2" t="inlineStr"/>
       <c r="E53" s="2" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
       </c>
       <c r="F53" s="2" t="n"/>
-      <c r="G53" s="2" t="b">
-        <v>1</v>
-      </c>
+      <c r="G53" s="2" t="n"/>
       <c r="H53" s="2" t="b">
         <v>1</v>
       </c>
@@ -5068,7 +5028,7 @@
         </is>
       </c>
       <c r="B60" s="2" t="n">
-        <v>68.12</v>
+        <v>0</v>
       </c>
       <c r="C60" s="2" t="n"/>
       <c r="D60" s="2" t="n"/>

</xml_diff>

<commit_message>
Redémarrage de Thunderbird après sauvegarde des mails Arrêt de Thunderbird au démarrage si la liste de contacts n'est pas créée Ajout d'une classe ProgressBarManager + widget caché quand pas utilisé et après 2.5s après fin progression Le statut des mails n'est plus enregistré dans le fichier .save mais est récupéré directement depuis Thunderbird Optimisation de la classe Save() Correction de 2 bugs : création ID unique pour les reçus et attribution du statut "DON-ADH" pour les RA Enregistrement automatique des contacts dans Thunderbird Début création de l'onglet "Options" Autres...
</commit_message>
<xml_diff>
--- a/donnees/listesAdherents/2024.xlsx
+++ b/donnees/listesAdherents/2024.xlsx
@@ -1867,7 +1867,7 @@
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>240105AR1;240110AR1</t>
+          <t>240105AR1;240110AR2</t>
         </is>
       </c>
       <c r="E18" s="2" t="inlineStr">
@@ -3304,7 +3304,7 @@
       </c>
       <c r="E36" s="2" t="inlineStr">
         <is>
-          <t>RA</t>
+          <t>DON-ADH</t>
         </is>
       </c>
       <c r="F36" s="2" t="n">
@@ -3921,12 +3921,12 @@
       </c>
       <c r="D44" s="2" t="inlineStr">
         <is>
-          <t>240123NP1</t>
+          <t>240123NP1;240123NP2</t>
         </is>
       </c>
       <c r="E44" s="2" t="inlineStr">
         <is>
-          <t>RA</t>
+          <t>DON-ADH</t>
         </is>
       </c>
       <c r="F44" s="2" t="n">
@@ -3964,10 +3964,10 @@
         <v>0</v>
       </c>
       <c r="P44" s="2" t="n">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="Q44" s="2" t="n">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="R44" s="2" t="inlineStr">
         <is>
@@ -4088,7 +4088,7 @@
       </c>
       <c r="E46" s="2" t="inlineStr">
         <is>
-          <t>RA</t>
+          <t>DON-ADH</t>
         </is>
       </c>
       <c r="F46" s="2" t="n">
@@ -4970,7 +4970,7 @@
         </is>
       </c>
       <c r="B58" s="2" t="n">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C58" s="2" t="n"/>
       <c r="D58" s="2" t="n"/>
@@ -4999,7 +4999,7 @@
         </is>
       </c>
       <c r="B59" s="2" t="n">
-        <v>6387.46</v>
+        <v>6402.46</v>
       </c>
       <c r="C59" s="2" t="n"/>
       <c r="D59" s="2" t="n"/>

</xml_diff>